<commit_message>
Updated layer definitions to use names from Staurenghi et al. 2014.
</commit_message>
<xml_diff>
--- a/data-raw/layer_definitions.xlsx
+++ b/data-raw/layer_definitions.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottwhitmore/stonelab/packages/heyexr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B196C2C-58CB-D141-B67A-5FFC8305C9EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="1320" windowWidth="28160" windowHeight="16880" tabRatio="500"/>
+    <workbookView xWindow="8780" yWindow="1320" windowWidth="28160" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IRA_v3.8.0" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -92,12 +93,6 @@
     <t>60.OPL-HFL_To_100.BMEIS</t>
   </si>
   <si>
-    <t>ONL-MZ</t>
-  </si>
-  <si>
-    <t>outer nuclear layer to myoid zone</t>
-  </si>
-  <si>
     <t>OPL-Henles fiber layer (OPL-HFL)</t>
   </si>
   <si>
@@ -107,33 +102,18 @@
     <t>EZ</t>
   </si>
   <si>
-    <t>ellipsoid zone of inner segment</t>
-  </si>
-  <si>
     <t>Boundary of myoid and ellipsoid of inner segments (BMEIS)</t>
   </si>
   <si>
     <t>110.IS/OSJ_To_120.IB_OPR</t>
   </si>
   <si>
-    <t>IZOS</t>
-  </si>
-  <si>
-    <t>inner zone of outer segment</t>
-  </si>
-  <si>
     <t>IS/OS junction (IS/OSJ)</t>
   </si>
   <si>
     <t>120.IB_OPR_To_140.IB_RPE</t>
   </si>
   <si>
-    <t>OZOS</t>
-  </si>
-  <si>
-    <t>outer zone of outer segment</t>
-  </si>
-  <si>
     <t>Inner boundary of OPR (IB_OPR)</t>
   </si>
   <si>
@@ -143,21 +123,12 @@
     <t>RPE</t>
   </si>
   <si>
-    <t>retinal pigment epithelium</t>
-  </si>
-  <si>
     <t>Inner boundary of RPE (IB_RPE)</t>
   </si>
   <si>
     <t>NA</t>
   </si>
   <si>
-    <t>outer RPE</t>
-  </si>
-  <si>
-    <t>outer boundary of RPE</t>
-  </si>
-  <si>
     <t>Outer boundary of RPE (OB_RPE)</t>
   </si>
   <si>
@@ -183,12 +154,42 @@
   </si>
   <si>
     <t>octexplorer_span</t>
+  </si>
+  <si>
+    <t>OS</t>
+  </si>
+  <si>
+    <t>IZ</t>
+  </si>
+  <si>
+    <t>CHOR-SCL</t>
+  </si>
+  <si>
+    <t>outer segments</t>
+  </si>
+  <si>
+    <t>interdigitation zone</t>
+  </si>
+  <si>
+    <t>ONL</t>
+  </si>
+  <si>
+    <t>Henle's fiber layer, outer nuclear layer, &amp; myoid zone</t>
+  </si>
+  <si>
+    <t>ellipsoid zone</t>
+  </si>
+  <si>
+    <t>RPE/Bruch's complex</t>
+  </si>
+  <si>
+    <t>choroid-sclera</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -230,21 +231,24 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G12" totalsRowShown="0">
-  <autoFilter ref="A1:G12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G12" totalsRowShown="0">
+  <autoFilter ref="A1:G12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
-    <tableColumn id="4" name="surface_id"/>
-    <tableColumn id="2" name="layer"/>
-    <tableColumn id="3" name="layer_description"/>
-    <tableColumn id="7" name="executable_surface_name"/>
-    <tableColumn id="1" name="octexplorer_span"/>
-    <tableColumn id="8" name="executable_name"/>
-    <tableColumn id="9" name="executable_version"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="surface_id"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="layer"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="layer_description"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="executable_surface_name"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="octexplorer_span"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="executable_name"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="executable_version"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -512,43 +516,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -568,10 +573,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -591,10 +596,10 @@
         <v>5</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -614,10 +619,10 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -637,10 +642,10 @@
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -660,10 +665,10 @@
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -671,22 +676,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -694,22 +699,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -717,22 +722,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -740,68 +745,68 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F10" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed numbering of layers. Added vitreous as a layer.
</commit_message>
<xml_diff>
--- a/data-raw/layer_definitions.xlsx
+++ b/data-raw/layer_definitions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottwhitmore/stonelab/packages/heyexr/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B196C2C-58CB-D141-B67A-5FFC8305C9EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C580E82-5829-9C41-8DBE-659702F5CD15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8780" yWindow="1320" windowWidth="28160" windowHeight="16880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>layer</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>choroid-sclera</t>
+  </si>
+  <si>
+    <t>VIT</t>
+  </si>
+  <si>
+    <t>vitreous</t>
   </si>
 </sst>
 </file>
@@ -239,8 +245,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G12" totalsRowShown="0">
-  <autoFilter ref="A1:G12" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:G13" totalsRowShown="0">
+  <autoFilter ref="A1:G13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="7">
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="surface_id"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="layer"/>
@@ -517,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,42 +564,42 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F3" t="s">
         <v>38</v>
@@ -604,19 +610,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
         <v>38</v>
@@ -627,19 +633,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
         <v>38</v>
@@ -650,19 +656,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
         <v>38</v>
@@ -673,19 +679,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
         <v>38</v>
@@ -696,19 +702,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
         <v>38</v>
@@ -719,19 +725,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
         <v>38</v>
@@ -742,19 +748,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
         <v>38</v>
@@ -765,19 +771,19 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F11" t="s">
         <v>38</v>
@@ -788,24 +794,47 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>52</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>33</v>
       </c>
-      <c r="F12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>